<commit_message>
Updates to Processing and figures
</commit_message>
<xml_diff>
--- a/processing_table.xlsx
+++ b/processing_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cawarmerdam/Documents/projects/lifelines_covid_research/umcg-rwarmerdam/analyses/qol_modelling_2022-12-12/covid19-qol-modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E6B90-83C0-8F4B-AC4F-FD924A3B7544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BAD3728-29F3-0A42-A630-FDA7F8B10D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{6BA91784-52AA-44DA-B804-53D1A43486FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{6BA91784-52AA-44DA-B804-53D1A43486FD}"/>
   </bookViews>
   <sheets>
     <sheet name="individual" sheetId="1" r:id="rId1"/>
@@ -165,24 +165,6 @@
     <t>General health</t>
   </si>
   <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>Neuroticism</t>
-  </si>
-  <si>
-    <t>Extraversion</t>
-  </si>
-  <si>
-    <t>Openness to experience</t>
-  </si>
-  <si>
-    <t>Agreeableness</t>
-  </si>
-  <si>
-    <t>Conscientiousness</t>
-  </si>
-  <si>
     <t>Beta</t>
   </si>
   <si>
@@ -292,6 +274,24 @@
   </si>
   <si>
     <t>{"10% lowest beta": "bottom", "10% lowest absolute beta": "around_zero", "10% highest beta": "top"}</t>
+  </si>
+  <si>
+    <t>Education (higher is more education)</t>
+  </si>
+  <si>
+    <t>Neuroticism (0 = agree, 21 = disagree)</t>
+  </si>
+  <si>
+    <t>Extraversion (0 = agree, 21 = disagree)</t>
+  </si>
+  <si>
+    <t>Openness to experience (0 = agree, 21 = disagree)</t>
+  </si>
+  <si>
+    <t>Agreeableness (0 = agree, 21 = disagree)</t>
+  </si>
+  <si>
+    <t>Conscientiousness (0 = agree, 20 = disagree)</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G21" sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,19 +739,19 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -762,42 +762,42 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -811,16 +811,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,16 +834,16 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,22 +851,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -874,22 +874,22 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,22 +897,22 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,22 +920,22 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -943,22 +943,22 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -966,22 +966,22 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -989,22 +989,22 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1012,22 +1012,22 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1035,22 +1035,22 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1058,22 +1058,22 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1081,22 +1081,22 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1104,68 +1104,68 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1173,22 +1173,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1196,22 +1196,22 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1244,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>23</v>
@@ -1255,7 +1255,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1263,7 +1263,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Corrected ordering to contain income mapping
</commit_message>
<xml_diff>
--- a/processing_table.xlsx
+++ b/processing_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cawarmerdam/Documents/projects/lifelines_covid_research/umcg-rwarmerdam/analyses/qol_modelling_2022-12-12/covid19-qol-modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BAD3728-29F3-0A42-A630-FDA7F8B10D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6459DA44-EF0C-C84D-B6D7-A2CC89F6748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{6BA91784-52AA-44DA-B804-53D1A43486FD}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>Generalized anxiety disorder</t>
   </si>
   <si>
-    <t>Gets COVID-19 related information and advice from traditional mass media outlets</t>
-  </si>
-  <si>
     <t>Gets COVID-19 related information and advice from health authorities</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>[9.0]</t>
   </si>
   <si>
-    <t>["&lt;€500", "€501-€1000", "€1001-€1500", "€1501-€2000", "€2001-€2500", "€2501-€3000", "€3001-€3500", "€3501-€4000", "€4001-€4500", "€4501-€5000", "€5001-€7500", "&gt;€7500"]</t>
-  </si>
-  <si>
     <t>filter</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>{}</t>
   </si>
   <si>
-    <t>["i prefer not to say"]</t>
-  </si>
-  <si>
     <t>{"yes":1, "no":0}</t>
   </si>
   <si>
@@ -292,6 +283,15 @@
   </si>
   <si>
     <t>Conscientiousness (0 = agree, 20 = disagree)</t>
+  </si>
+  <si>
+    <t>Gets COVID-19 related information and advice from traditional media outlets</t>
+  </si>
+  <si>
+    <t>{"i prefer not to say":13}</t>
+  </si>
+  <si>
+    <t>{"&lt;€500":1, "€501-€1000":2, "€1001-€1500":3, "€1501-€2000":4, "€2001-€2500":5, "€2501-€3000":6, "€3001-€3500":7, "€3501-€4000":8, "€4001-€4500":9, "€4501-€5000":10, "€5001-€7500":11, "&gt;€7500":12}</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G21" sqref="A1:G21"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,16 +739,16 @@
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>50</v>
@@ -762,42 +762,42 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -811,16 +811,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>51</v>
@@ -843,7 +843,7 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -851,22 +851,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -874,22 +874,22 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
         <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -897,22 +897,22 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -920,22 +920,22 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -943,22 +943,22 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
         <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -966,22 +966,22 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -989,22 +989,22 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1012,16 +1012,16 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1035,16 +1035,16 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1058,16 +1058,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -1081,16 +1081,16 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -1104,16 +1104,16 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -1133,16 +1133,16 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1156,16 +1156,16 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1176,19 +1176,19 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1199,19 +1199,19 @@
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>